<commit_message>
data and notebook update
</commit_message>
<xml_diff>
--- a/dash-2019-coronavirus/data.xlsx
+++ b/dash-2019-coronavirus/data.xlsx
@@ -8,31 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/Dropbox/Course/data-visualisation-scripts/dash-2019-coronavirus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EAECEE-EF9B-BA43-B7CB-72485B1B505B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECFC815-89DD-5844-94B1-7216C26F3A46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6680" yWindow="1360" windowWidth="32760" windowHeight="19260" xr2:uid="{66589947-9D93-AC48-8CDC-7FAFDE9EADB7}"/>
   </bookViews>
   <sheets>
-    <sheet name="2020-01-30-11-00" sheetId="20" r:id="rId1"/>
-    <sheet name="2020-01-29-21-00" sheetId="19" r:id="rId2"/>
-    <sheet name="2020-01-29-14-30" sheetId="18" r:id="rId3"/>
-    <sheet name="2020-01-29-13-00" sheetId="17" r:id="rId4"/>
-    <sheet name="2020-01-28-23-00" sheetId="16" r:id="rId5"/>
-    <sheet name="2020-01-28-18-00" sheetId="15" r:id="rId6"/>
-    <sheet name="2020-01-28-13-00" sheetId="14" r:id="rId7"/>
-    <sheet name="2020-01-27-20-30" sheetId="1" r:id="rId8"/>
-    <sheet name="2020-01-27-19-00" sheetId="2" r:id="rId9"/>
-    <sheet name="2020-01-27-09-00" sheetId="3" r:id="rId10"/>
-    <sheet name="2020-01-26-23-00" sheetId="4" r:id="rId11"/>
-    <sheet name="2020-01-26-11-00" sheetId="5" r:id="rId12"/>
-    <sheet name="2020-01-25-22-00" sheetId="6" r:id="rId13"/>
-    <sheet name="2020-01-25-12-00" sheetId="7" r:id="rId14"/>
-    <sheet name="2020-01-25-00-00" sheetId="8" r:id="rId15"/>
-    <sheet name="2020-01-24-12-00" sheetId="9" r:id="rId16"/>
-    <sheet name="2020-01-24-00-00" sheetId="10" r:id="rId17"/>
-    <sheet name="2020-01-23-12-00" sheetId="11" r:id="rId18"/>
-    <sheet name="2020-01-22-12-00" sheetId="12" r:id="rId19"/>
-    <sheet name="2020-01-22-00-00" sheetId="13" r:id="rId20"/>
+    <sheet name="2020-01-30-21-30" sheetId="21" r:id="rId1"/>
+    <sheet name="2020-01-30-11-00" sheetId="20" r:id="rId2"/>
+    <sheet name="2020-01-29-21-00" sheetId="19" r:id="rId3"/>
+    <sheet name="2020-01-29-14-30" sheetId="18" r:id="rId4"/>
+    <sheet name="2020-01-29-13-00" sheetId="17" r:id="rId5"/>
+    <sheet name="2020-01-28-23-00" sheetId="16" r:id="rId6"/>
+    <sheet name="2020-01-28-18-00" sheetId="15" r:id="rId7"/>
+    <sheet name="2020-01-28-13-00" sheetId="14" r:id="rId8"/>
+    <sheet name="2020-01-27-20-30" sheetId="1" r:id="rId9"/>
+    <sheet name="2020-01-27-19-00" sheetId="2" r:id="rId10"/>
+    <sheet name="2020-01-27-09-00" sheetId="3" r:id="rId11"/>
+    <sheet name="2020-01-26-23-00" sheetId="4" r:id="rId12"/>
+    <sheet name="2020-01-26-11-00" sheetId="5" r:id="rId13"/>
+    <sheet name="2020-01-25-22-00" sheetId="6" r:id="rId14"/>
+    <sheet name="2020-01-25-12-00" sheetId="7" r:id="rId15"/>
+    <sheet name="2020-01-25-00-00" sheetId="8" r:id="rId16"/>
+    <sheet name="2020-01-24-12-00" sheetId="9" r:id="rId17"/>
+    <sheet name="2020-01-24-00-00" sheetId="10" r:id="rId18"/>
+    <sheet name="2020-01-23-12-00" sheetId="11" r:id="rId19"/>
+    <sheet name="2020-01-22-12-00" sheetId="12" r:id="rId20"/>
+    <sheet name="2020-01-22-00-00" sheetId="13" r:id="rId21"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="117">
   <si>
     <t>Province/State</t>
   </si>
@@ -389,6 +390,12 @@
   </si>
   <si>
     <t>India</t>
+  </si>
+  <si>
+    <t>1/30/2020 21:30</t>
+  </si>
+  <si>
+    <t>Italy</t>
   </si>
 </sst>
 </file>
@@ -760,8 +767,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A92FA9-C4D2-D54D-A858-31DC22BED2E4}">
-  <dimension ref="A1:F59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588C3779-7322-B347-9AEE-79E794B2FD63}">
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A1048576"/>
@@ -797,16 +804,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D2" s="1">
-        <v>4903</v>
+        <v>5806</v>
       </c>
       <c r="E2" s="1">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="F2" s="1">
-        <v>90</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -817,14 +824,14 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D3" s="1">
-        <v>428</v>
+        <v>537</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -835,14 +842,14 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D4" s="1">
-        <v>354</v>
+        <v>393</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -853,16 +860,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D5" s="1">
-        <v>278</v>
+        <v>352</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -873,10 +880,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D6" s="1">
-        <v>277</v>
+        <v>332</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1">
@@ -885,56 +892,56 @@
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D7" s="1">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D8" s="1">
-        <v>182</v>
+        <v>237</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D9" s="1">
-        <v>162</v>
+        <v>206</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -945,14 +952,14 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D10" s="1">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -963,10 +970,10 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D11" s="1">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -983,48 +990,48 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D12" s="1">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D13" s="1">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D14" s="1">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
@@ -1041,7 +1048,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D15" s="1">
         <v>101</v>
@@ -1057,10 +1064,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D16" s="1">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="1">
@@ -1069,36 +1076,36 @@
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D17" s="1">
-        <v>70</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D18" s="1">
-        <v>65</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1109,51 +1116,51 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D19" s="1">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="1">
+        <v>59</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20" s="1">
-        <v>46</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D21" s="1">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E21" s="1">
-        <v>2</v>
-      </c>
-      <c r="F21" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -1163,10 +1170,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D22" s="1">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="1">
@@ -1181,10 +1188,10 @@
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D23" s="1">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="1">
@@ -1199,10 +1206,10 @@
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D24" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1215,92 +1222,94 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D25" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D26" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D27" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
     <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D28" s="1">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="1">
-        <v>1</v>
-      </c>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D29" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D30" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="1">
@@ -1315,10 +1324,10 @@
         <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D31" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1331,7 +1340,7 @@
         <v>39</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D32" s="1">
         <v>9</v>
@@ -1347,7 +1356,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D33" s="1">
         <v>8</v>
@@ -1363,7 +1372,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D34" s="1">
         <v>7</v>
@@ -1379,7 +1388,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -1395,7 +1404,7 @@
         <v>42</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
@@ -1411,10 +1420,10 @@
         <v>42</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -1427,7 +1436,7 @@
         <v>42</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D38" s="1">
         <v>2</v>
@@ -1443,7 +1452,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
@@ -1457,7 +1466,7 @@
         <v>46</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D40" s="1">
         <v>11</v>
@@ -1473,7 +1482,7 @@
         <v>47</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D41" s="1">
         <v>14</v>
@@ -1489,10 +1498,10 @@
         <v>48</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D42" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -1503,7 +1512,7 @@
         <v>49</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D43" s="1">
         <v>10</v>
@@ -1517,7 +1526,7 @@
         <v>50</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D44" s="1">
         <v>2</v>
@@ -1531,7 +1540,7 @@
         <v>51</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D45" s="1">
         <v>5</v>
@@ -1545,7 +1554,7 @@
         <v>52</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
@@ -1559,7 +1568,7 @@
         <v>53</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D47" s="1">
         <v>8</v>
@@ -1575,7 +1584,7 @@
         <v>55</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D48" s="1">
         <v>2</v>
@@ -1591,7 +1600,7 @@
         <v>55</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
@@ -1605,7 +1614,7 @@
         <v>56</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
@@ -1619,7 +1628,7 @@
         <v>57</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
@@ -1635,7 +1644,7 @@
         <v>60</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D52" s="1">
         <v>4</v>
@@ -1653,7 +1662,7 @@
         <v>60</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D53" s="1">
         <v>2</v>
@@ -1669,7 +1678,7 @@
         <v>60</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D54" s="1">
         <v>3</v>
@@ -1685,7 +1694,7 @@
         <v>63</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D55" s="1">
         <v>4</v>
@@ -1699,7 +1708,7 @@
         <v>102</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
@@ -1713,7 +1722,7 @@
         <v>100</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D57" s="1">
         <v>4</v>
@@ -1727,7 +1736,7 @@
         <v>70</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
@@ -1741,11 +1750,26 @@
         <v>114</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
       </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+      <c r="B60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" s="1">
+        <v>2</v>
+      </c>
+      <c r="E60" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1753,6 +1777,869 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1F0C4D-014C-9646-864D-4C2E0D15963F}">
+  <dimension ref="A1:F52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1423</v>
+      </c>
+      <c r="E2" s="1">
+        <v>76</v>
+      </c>
+      <c r="F2" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="1">
+        <v>151</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="1">
+        <v>128</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1">
+        <v>128</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1">
+        <v>110</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="1">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1">
+        <v>80</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1">
+        <v>72</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="1">
+        <v>70</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1">
+        <v>69</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1">
+        <v>59</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="1">
+        <v>53</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1">
+        <v>47</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1">
+        <v>35</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="1">
+        <v>33</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="1">
+        <v>27</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="1">
+        <v>26</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="1">
+        <v>23</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="1">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="1">
+        <v>18</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1">
+        <v>14</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1">
+        <v>13</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="1">
+        <v>11</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="1">
+        <v>7</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="1">
+        <v>6</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="1">
+        <v>6</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="1">
+        <v>5</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="1">
+        <v>5</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="1">
+        <v>2</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="1">
+        <v>1</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="1">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="1">
+        <v>8</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="1">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="1">
+        <v>5</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="1">
+        <v>4</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" s="1">
+        <v>4</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="1">
+        <v>1</v>
+      </c>
+      <c r="E52" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55474FAD-47BE-A446-80F0-0652C8024DDE}">
   <dimension ref="A1:F49"/>
   <sheetViews>
@@ -2567,7 +3454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D109F2-335E-B842-B29F-32988756D99B}">
   <dimension ref="A1:F48"/>
   <sheetViews>
@@ -3364,7 +4251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422DC1B8-61A7-9F4B-AD6D-16910AF9DAD2}">
   <dimension ref="A1:G47"/>
   <sheetViews>
@@ -4208,7 +5095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C14E1D-A573-C549-91F0-85D6781C45FF}">
   <dimension ref="A1:G45"/>
   <sheetViews>
@@ -5016,7 +5903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF828E8-2C21-3145-94D4-8BD2B2FC2D5C}">
   <dimension ref="A1:G45"/>
   <sheetViews>
@@ -5820,7 +6707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74C6ACE-A5E7-894A-9E03-A4D184028106}">
   <dimension ref="A1:G45"/>
   <sheetViews>
@@ -6622,7 +7509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F996331F-AA5D-7040-8F17-DE10C3DA49A5}">
   <dimension ref="A1:G42"/>
   <sheetViews>
@@ -7383,7 +8270,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459AF105-9E29-6E4D-801B-CA0BFB7BA013}">
   <dimension ref="A1:G39"/>
   <sheetViews>
@@ -8087,7 +8974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4DD976-0303-C747-BFEB-22EC0C288A7A}">
   <dimension ref="A1:G47"/>
   <sheetViews>
@@ -8895,7 +9782,1000 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A92FA9-C4D2-D54D-A858-31DC22BED2E4}">
+  <dimension ref="A1:F59"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4903</v>
+      </c>
+      <c r="E2" s="1">
+        <v>162</v>
+      </c>
+      <c r="F2" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="1">
+        <v>428</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="1">
+        <v>354</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="1">
+        <v>278</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="1">
+        <v>277</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="1">
+        <v>200</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="1">
+        <v>182</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="1">
+        <v>162</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="1">
+        <v>158</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D11" s="1">
+        <v>142</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="1">
+        <v>129</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="1">
+        <v>114</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="1">
+        <v>112</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="1">
+        <v>101</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="1">
+        <v>78</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="1">
+        <v>70</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" s="1">
+        <v>65</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="1">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="1">
+        <v>46</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="1">
+        <v>44</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="1">
+        <v>41</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="1">
+        <v>35</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="1">
+        <v>31</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="1">
+        <v>26</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="1">
+        <v>19</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="1">
+        <v>17</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="1">
+        <v>14</v>
+      </c>
+      <c r="E28" s="2"/>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="1">
+        <v>14</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="1">
+        <v>12</v>
+      </c>
+      <c r="E30" s="2"/>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="1">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="1">
+        <v>9</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="1">
+        <v>8</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="1">
+        <v>7</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="1">
+        <v>2</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="1">
+        <v>11</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="1">
+        <v>14</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="1">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="1">
+        <v>10</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" s="1">
+        <v>8</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D48" s="1">
+        <v>2</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" s="1">
+        <v>1</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="1">
+        <v>4</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="1">
+        <v>2</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D55" s="1">
+        <v>4</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="2"/>
+      <c r="B56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="2"/>
+      <c r="B57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="1">
+        <v>4</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="2"/>
+      <c r="B58" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="1">
+        <v>1</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="2"/>
+      <c r="B59" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5045D7-534A-2941-A13E-3353E7C989D0}">
   <dimension ref="A1:G39"/>
   <sheetViews>
@@ -9497,7 +11377,456 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3B2472-BF00-6D4E-8BC5-C6308F1CA7BB}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C2:C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="1">
+        <v>17</v>
+      </c>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="1">
+        <v>270</v>
+      </c>
+      <c r="G18" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="G23" s="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="1">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="2"/>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33442B0-0FCD-C24F-82A7-97538A6C6A0F}">
   <dimension ref="A1:F57"/>
   <sheetViews>
@@ -10459,456 +12788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3B2472-BF00-6D4E-8BC5-C6308F1CA7BB}">
-  <dimension ref="A1:G28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C2:C28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="1">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="1">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="G10" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="1">
-        <v>17</v>
-      </c>
-      <c r="G12" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="1">
-        <v>5</v>
-      </c>
-      <c r="G16" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="1">
-        <v>270</v>
-      </c>
-      <c r="G18" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="G20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="G21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="1">
-        <v>5</v>
-      </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="G23" s="1">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="G24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="1">
-        <v>2</v>
-      </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE09DF1A-6004-3F41-87FE-5242A451DCFE}">
   <dimension ref="A1:F55"/>
   <sheetViews>
@@ -11841,7 +13721,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CB9813-8C08-1D4E-84D9-F0E88353F568}">
   <dimension ref="A1:F53"/>
   <sheetViews>
@@ -12730,7 +14610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA30479F-90F4-334C-8C59-590760A6FAA8}">
   <dimension ref="A1:F53"/>
   <sheetViews>
@@ -13617,7 +15497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E060AD5B-754C-1E4C-BB87-BCC5A5BA20D5}">
   <dimension ref="A1:G53"/>
   <sheetViews>
@@ -14659,7 +16539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B466029B-456E-124B-9B1A-E6BFF4A8E651}">
   <dimension ref="A1:F52"/>
   <sheetViews>
@@ -15526,7 +17406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B042FB-9034-D541-B348-29085FA9B6CC}">
   <dimension ref="A1:F53"/>
   <sheetViews>
@@ -16408,867 +18288,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1F0C4D-014C-9646-864D-4C2E0D15963F}">
-  <dimension ref="A1:F52"/>
-  <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1423</v>
-      </c>
-      <c r="E2" s="1">
-        <v>76</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="1">
-        <v>151</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="1">
-        <v>128</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="1">
-        <v>128</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="1">
-        <v>110</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="1">
-        <v>100</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="1">
-        <v>80</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="1">
-        <v>75</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="1">
-        <v>72</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="1">
-        <v>70</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="1">
-        <v>69</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="1">
-        <v>59</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="1">
-        <v>53</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="1">
-        <v>47</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="1">
-        <v>46</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="1">
-        <v>35</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="1">
-        <v>33</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="1">
-        <v>27</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="1">
-        <v>26</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D21" s="1">
-        <v>23</v>
-      </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="1">
-        <v>21</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="1">
-        <v>18</v>
-      </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" s="1">
-        <v>14</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="1">
-        <v>13</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="1">
-        <v>11</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="1">
-        <v>8</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D28" s="1">
-        <v>7</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D29" s="1">
-        <v>7</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="1">
-        <v>6</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="1">
-        <v>6</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="1">
-        <v>6</v>
-      </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="1">
-        <v>5</v>
-      </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="1">
-        <v>5</v>
-      </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-    </row>
-    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="1">
-        <v>1</v>
-      </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D36" s="1">
-        <v>1</v>
-      </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="1">
-        <v>2</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1</v>
-      </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D39" s="1">
-        <v>4</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D40" s="1">
-        <v>8</v>
-      </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D41" s="1">
-        <v>4</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-    </row>
-    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="1">
-        <v>5</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D43" s="1">
-        <v>2</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="1">
-        <v>3</v>
-      </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="1">
-        <v>1</v>
-      </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D46" s="1">
-        <v>4</v>
-      </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" s="1">
-        <v>1</v>
-      </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="2"/>
-      <c r="B48" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="1">
-        <v>1</v>
-      </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-    </row>
-    <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="2"/>
-      <c r="B49" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D49" s="1">
-        <v>1</v>
-      </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-    </row>
-    <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-      <c r="B50" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-    </row>
-    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D51" s="1">
-        <v>4</v>
-      </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-    </row>
-    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D52" s="1">
-        <v>1</v>
-      </c>
-      <c r="E52" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>